<commit_message>
Add RailsImporter::Base spec along with module specs
Also ImportJob specs were added.
</commit_message>
<xml_diff>
--- a/lib/rails_importer/templates/importer.xlsx
+++ b/lib/rails_importer/templates/importer.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sivicencio/Documents/code/rails_importer/lib/rails_importer/templates/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,6 +21,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>importer</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -57,6 +73,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -382,17 +403,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>